<commit_message>
save all work before I change stuff to account for the PLM error and thus of new fafb
</commit_message>
<xml_diff>
--- a/literature/record_oscillations.xlsx
+++ b/literature/record_oscillations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-27360" yWindow="820" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Record of oscillations in the learning literature</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>precise citation on the previous:</t>
+  </si>
+  <si>
+    <t>Clarida, Gali, Gertler 1999</t>
+  </si>
+  <si>
+    <t>p. 1701</t>
+  </si>
+  <si>
+    <t>"… if the rule calls for an overly aggressive response of interest rates to movements in expected inflation. In this instance, there is a 'policy overkill' effect that emerges and may result in an oscillating equilibrium."</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,6 +615,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
woodford noninertial optimal plan, Peter meeting
</commit_message>
<xml_diff>
--- a/literature/record_oscillations.xlsx
+++ b/literature/record_oscillations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Record of oscillations in the learning literature</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>"… if the rule calls for an overly aggressive response of interest rates to movements in expected inflation. In this instance, there is a 'policy overkill' effect that emerges and may result in an oscillating equilibrium."</t>
+  </si>
+  <si>
+    <t>Evans Honkapohja 2001</t>
+  </si>
+  <si>
+    <t>p. 41</t>
+  </si>
+  <si>
+    <t>overparameterization of PLM</t>
   </si>
 </sst>
 </file>
@@ -511,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -626,6 +635,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
reading, Alpha Chiang work, Woodford
</commit_message>
<xml_diff>
--- a/literature/record_oscillations.xlsx
+++ b/literature/record_oscillations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Record of oscillations in the learning literature</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>"a policy of strongly responding to variations in expected inflation as a way of preventing such fluctuations can be counterproductive, as it may actually enable instability of inflation due to self-fulfilling expectations. (See also Proposition 7.13.)"</t>
+  </si>
+  <si>
+    <t>Branch 2004 restricted</t>
+  </si>
+  <si>
+    <t>p.4</t>
+  </si>
+  <si>
+    <t>"negative feedback from expectations. This particular self-referential feature generates expectations driven oscillations."</t>
   </si>
 </sst>
 </file>
@@ -536,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -674,6 +683,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
incroporated Woodford finite planning and anchor and adjustment reference into draft 2
</commit_message>
<xml_diff>
--- a/literature/record_oscillations.xlsx
+++ b/literature/record_oscillations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27360" yWindow="820" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Record of oscillations in the learning literature</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>"negative feedback from expectations. This particular self-referential feature generates expectations driven oscillations."</t>
+  </si>
+  <si>
+    <t>Hommes 2019/20 JEL</t>
+  </si>
+  <si>
+    <t>oscillation under positive feedback</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -694,6 +700,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>